<commit_message>
Comments and clean up
</commit_message>
<xml_diff>
--- a/Archive/20240430_Dataset.xlsx
+++ b/Archive/20240430_Dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabiansauer/GitHub/FluffFinder/Archive/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B42F02A5-ADE0-1E4E-982A-D7C06680126C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD4A0429-1221-1646-BD12-444190782DBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{13578E20-B2CD-4D40-B27D-694AA7ED1355}"/>
+    <workbookView xWindow="40" yWindow="1080" windowWidth="28800" windowHeight="16600" xr2:uid="{13578E20-B2CD-4D40-B27D-694AA7ED1355}"/>
   </bookViews>
   <sheets>
     <sheet name="Dataset" sheetId="1" r:id="rId1"/>
@@ -1368,7 +1368,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1417,18 +1417,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="14">
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1577,6 +1571,9 @@
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1594,33 +1591,33 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C4092E84-7EFB-E547-B240-FBFF29DF5637}" name="Table2" displayName="Table2" ref="A1:E91" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A1:E91" xr:uid="{23FACA8B-8412-E443-BCAD-74DE1B4DAB42}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{0D12865F-30AF-C448-A078-71768EFE9428}" name="Index" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{63BE7029-CDB1-B346-9DDD-6A64AD7ECBE5}" name="Industry" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{92245087-302D-0B4C-B8C6-18E73BE17143}" name="Interest Category" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{4F70FEE5-DE31-BE47-95DB-A96F3F1A8CE2}" name="Text" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{40BE8989-ED6E-9248-A608-F217048025B4}" name="URL" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{0D12865F-30AF-C448-A078-71768EFE9428}" name="Index" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{63BE7029-CDB1-B346-9DDD-6A64AD7ECBE5}" name="Industry" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{92245087-302D-0B4C-B8C6-18E73BE17143}" name="Interest Category" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{4F70FEE5-DE31-BE47-95DB-A96F3F1A8CE2}" name="Text" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{40BE8989-ED6E-9248-A608-F217048025B4}" name="URL" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{713C2A9D-8E5B-D548-96EB-68F7B2C08198}" name="Table3" displayName="Table3" ref="A1:C7" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{713C2A9D-8E5B-D548-96EB-68F7B2C08198}" name="Table3" displayName="Table3" ref="A1:C7" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A1:C7" xr:uid="{713C2A9D-8E5B-D548-96EB-68F7B2C08198}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{F7960138-DACE-D244-98DE-21EE51418E90}" name="Interest Category" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{854023F7-CB45-4845-9FC3-1DD7C8AA1E9D}" name="Description" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{D2FB778B-3802-6949-8F56-4AB3E609F7E5}" name="Criteria" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{F7960138-DACE-D244-98DE-21EE51418E90}" name="Interest Category" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{854023F7-CB45-4845-9FC3-1DD7C8AA1E9D}" name="Description" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{D2FB778B-3802-6949-8F56-4AB3E609F7E5}" name="Criteria" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6163F8CD-161F-6F43-840F-CCCF5208C939}" name="Table1" displayName="Table1" ref="B2:B5" totalsRowShown="0" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6163F8CD-161F-6F43-840F-CCCF5208C939}" name="Table1" displayName="Table1" ref="B2:B5" totalsRowShown="0" dataDxfId="1">
   <autoFilter ref="B2:B5" xr:uid="{6163F8CD-161F-6F43-840F-CCCF5208C939}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{C94C76A5-C7E2-A04A-88C7-31075D906035}" name="Checks" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{C94C76A5-C7E2-A04A-88C7-31075D906035}" name="Checks" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1945,8 +1942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7685544D-B518-AF41-B6B6-92A3EDD35CF5}">
   <dimension ref="A1:E91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79:C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3176,7 +3173,7 @@
       <c r="C72" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D72" s="18" t="s">
+      <c r="D72" s="2" t="s">
         <v>217</v>
       </c>
       <c r="E72" s="6" t="s">
@@ -3586,6 +3583,7 @@
     <hyperlink ref="E91" r:id="rId76" xr:uid="{57856EBE-1FA0-B647-92E3-627A23898876}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId77"/>
   </tableParts>

</xml_diff>